<commit_message>
problem 2 probably solved, need special mutation strategy
</commit_message>
<xml_diff>
--- a/problem 3 - concept/jobs.xlsx
+++ b/problem 3 - concept/jobs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deric\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deric\Desktop\ai-genetic\ai-projet2-genetic\problem 3 - concept\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5014520-4BCE-4EE5-AF90-0841F5F8760D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B14940-D714-409E-9E13-B6498BD774BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{2134C11B-C8CC-4877-9366-45380615B26B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
   <si>
     <t>JOB TITLE</t>
   </si>
@@ -173,6 +173,21 @@
   </si>
   <si>
     <t>Artist</t>
+  </si>
+  <si>
+    <t>Une intersection : l'impact dans la matrice de satisfaction globale</t>
+  </si>
+  <si>
+    <t>CHACUN DES COLONNES DONNE UN SCORE DE 1</t>
+  </si>
+  <si>
+    <t>TOTAL (1)</t>
+  </si>
+  <si>
+    <t>PONDÉRATION (Variable contexte)</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -228,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -245,8 +260,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -562,38 +586,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7D3F53-E2D2-416E-AD93-0175C9D788F7}">
-  <dimension ref="A1:P53"/>
+  <dimension ref="A1:P54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="16" width="17.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21" style="3" customWidth="1"/>
+    <col min="3" max="16" width="17.7109375" style="3" customWidth="1"/>
     <col min="17" max="20" width="16.7109375" customWidth="1"/>
     <col min="21" max="21" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
     </row>
     <row r="2" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -626,7 +651,9 @@
       <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="2"/>
+      <c r="K2" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -709,7 +736,7 @@
         <v>37</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>10</v>
@@ -860,7 +887,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
@@ -877,13 +904,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="D18" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="H18" s="3" t="s">
         <v>18</v>
       </c>
@@ -894,51 +924,127 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="C19" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="D19" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="6">
+        <v>1</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1</v>
+      </c>
+      <c r="D20" s="6">
+        <v>1</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1</v>
+      </c>
+      <c r="F20" s="6">
+        <v>1</v>
+      </c>
+      <c r="G20" s="6">
+        <v>1</v>
+      </c>
+      <c r="H20" s="6">
+        <v>1</v>
+      </c>
+      <c r="I20" s="6">
+        <v>1</v>
+      </c>
+      <c r="J20" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
@@ -1004,9 +1110,14 @@
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
     </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:O1"/>
+    <mergeCell ref="B22:I23"/>
+    <mergeCell ref="B24:I24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update on jobs excel
</commit_message>
<xml_diff>
--- a/problem 3 - concept/jobs.xlsx
+++ b/problem 3 - concept/jobs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deric\Desktop\ai-genetic\ai-projet2-genetic\problem 3 - concept\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B14940-D714-409E-9E13-B6498BD774BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA76AD13-4BCC-48F5-B87A-D16B22538B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{2134C11B-C8CC-4877-9366-45380615B26B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="63">
   <si>
     <t>JOB TITLE</t>
   </si>
@@ -188,13 +188,52 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>VERSION SIMPLIFIÉE (POINT DE DÉPART)</t>
+  </si>
+  <si>
+    <t>Doctor [0]</t>
+  </si>
+  <si>
+    <t>Engineer [1]</t>
+  </si>
+  <si>
+    <t>Farmer [2]</t>
+  </si>
+  <si>
+    <t>Worker [3]</t>
+  </si>
+  <si>
+    <t>COMMUNITY COST[0]</t>
+  </si>
+  <si>
+    <t>FOOD PRODUCTION[1]</t>
+  </si>
+  <si>
+    <t>GOODS PRODUCTION[2]</t>
+  </si>
+  <si>
+    <t>HEALTH[3]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ex : En temps de paix et de croissance économique, on se soucie moins d'avoir un gros Community Cost. En temps de guerre, c'est le contraire </t>
+  </si>
+  <si>
+    <t>CONTEXTE DE BASE: Stable, croissance économique, population vieillissante</t>
+  </si>
+  <si>
+    <t>PONDÉRATION (Variable selon contexte)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,8 +249,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="6" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,6 +310,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -243,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -260,17 +364,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -588,15 +740,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7D3F53-E2D2-416E-AD93-0175C9D788F7}">
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21" style="3" customWidth="1"/>
-    <col min="3" max="16" width="17.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" style="3" customWidth="1"/>
+    <col min="6" max="16" width="17.7109375" style="3" customWidth="1"/>
     <col min="17" max="20" width="16.7109375" customWidth="1"/>
     <col min="21" max="21" width="12.7109375" customWidth="1"/>
   </cols>
@@ -664,329 +819,425 @@
       <c r="A3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="12" t="s">
         <v>10</v>
       </c>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="13">
+        <v>0</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="E4" s="12"/>
+      <c r="F4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="H4" s="12"/>
+      <c r="I4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="12" t="s">
         <v>19</v>
       </c>
+      <c r="K4" s="12"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12" t="s">
         <v>32</v>
       </c>
+      <c r="K5" s="12"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12">
         <v>1</v>
       </c>
-      <c r="E6" s="3">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="12" t="s">
         <v>22</v>
       </c>
+      <c r="K6" s="12"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="12" t="s">
         <v>16</v>
       </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3">
+      <c r="B8" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="C8" s="12">
         <v>1</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12" t="s">
         <v>15</v>
       </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="12" t="s">
         <v>30</v>
       </c>
+      <c r="K9" s="12"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="14" t="s">
         <v>40</v>
       </c>
+      <c r="K10" s="12"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="K11" s="12"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="B12" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="H12" s="12"/>
+      <c r="I12" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="J12" s="14" t="s">
         <v>22</v>
       </c>
+      <c r="K12" s="12"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J13" s="5"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="12"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="K14" s="12"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" s="3" t="s">
+      <c r="B15" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="H15" s="12"/>
+      <c r="I15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="J15" s="12" t="s">
         <v>18</v>
       </c>
+      <c r="K15" s="12"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="3" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="H16" s="12"/>
+      <c r="I16" s="12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="3" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="J17" s="12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="12"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="3" t="s">
+      <c r="I18" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="12"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="B19" s="13">
+        <v>0</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="15">
+        <f>SUM(B4:B19)</f>
+        <v>0.8</v>
+      </c>
+      <c r="C20" s="16">
         <v>1</v>
       </c>
-      <c r="C20" s="6">
+      <c r="D20" s="16">
         <v>1</v>
       </c>
-      <c r="D20" s="6">
+      <c r="E20" s="16">
         <v>1</v>
       </c>
-      <c r="E20" s="6">
+      <c r="F20" s="16">
         <v>1</v>
       </c>
-      <c r="F20" s="6">
+      <c r="G20" s="16">
         <v>1</v>
       </c>
-      <c r="G20" s="6">
+      <c r="H20" s="16">
         <v>1</v>
       </c>
-      <c r="H20" s="6">
+      <c r="I20" s="16">
         <v>1</v>
       </c>
-      <c r="I20" s="6">
+      <c r="J20" s="16">
         <v>1</v>
       </c>
-      <c r="J20" s="6">
+      <c r="K20" s="12"/>
+    </row>
+    <row r="21" spans="1:16" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="9" t="s">
         <v>46</v>
@@ -999,7 +1250,7 @@
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -1010,7 +1261,7 @@
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="9" t="s">
         <v>47</v>
@@ -1023,76 +1274,220 @@
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" s="19" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="C28" s="20">
+        <v>0</v>
+      </c>
+      <c r="D28" s="20">
+        <v>0</v>
+      </c>
+      <c r="E28" s="20">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="20">
+        <v>0.375</v>
+      </c>
+      <c r="C29" s="20">
+        <v>0.15</v>
+      </c>
+      <c r="D29" s="20">
+        <v>0.35</v>
+      </c>
+      <c r="E29" s="20">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="C30" s="20">
+        <v>0.6</v>
+      </c>
+      <c r="D30" s="20">
+        <v>0</v>
+      </c>
+      <c r="E30" s="20">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="20">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C31" s="20">
+        <v>0.25</v>
+      </c>
+      <c r="D31" s="20">
+        <v>0.65</v>
+      </c>
+      <c r="E31" s="20">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="22">
+        <f>SUM(B28:B31)</f>
+        <v>1</v>
+      </c>
+      <c r="C33" s="22">
+        <f>SUM(C28:C31)</f>
+        <v>1</v>
+      </c>
+      <c r="D33" s="22">
+        <f>SUM(D28:D31)</f>
+        <v>1</v>
+      </c>
+      <c r="E33" s="22">
+        <f>SUM(E28:E31)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="C34" s="23">
+        <v>0.2</v>
+      </c>
+      <c r="D34" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="E34" s="23">
+        <v>0.4</v>
+      </c>
+      <c r="F34" s="21">
+        <f>SUM(B34:E34)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
@@ -1114,10 +1509,11 @@
       <c r="A54" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="B22:I23"/>
     <mergeCell ref="B24:I24"/>
+    <mergeCell ref="B25:K25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1125,15 +1521,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010006B233B9B3A5024C99847B1D0443027F" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="39a3a9a18fc0038d1c425abb13176a98">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d59a1f78-4cdc-402c-b8a0-58bfb80633d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="635a148d9eedb07babeb6ca05c95a7d9" ns3:_="">
     <xsd:import namespace="d59a1f78-4cdc-402c-b8a0-58bfb80633d0"/>
@@ -1265,6 +1652,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1272,14 +1668,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F3EA1CF-A27A-4CFA-9674-6A86EB7CE3B7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D72B6365-5724-4DCC-8EE2-F84342C5EBFF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1293,6 +1681,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F3EA1CF-A27A-4CFA-9674-6A86EB7CE3B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
work on Excel + start coding Happy Problem
</commit_message>
<xml_diff>
--- a/problem 3 - concept/jobs.xlsx
+++ b/problem 3 - concept/jobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deric\Desktop\ai-genetic\ai-projet2-genetic\problem 3 - concept\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA76AD13-4BCC-48F5-B87A-D16B22538B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A5E260-3EDB-48CF-AE71-DB1F38D7ABA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{2134C11B-C8CC-4877-9366-45380615B26B}"/>
+    <workbookView xWindow="10920" yWindow="1080" windowWidth="28785" windowHeight="14505" xr2:uid="{2134C11B-C8CC-4877-9366-45380615B26B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
   <si>
     <t>JOB TITLE</t>
   </si>
@@ -220,10 +220,28 @@
     <t xml:space="preserve">Ex : En temps de paix et de croissance économique, on se soucie moins d'avoir un gros Community Cost. En temps de guerre, c'est le contraire </t>
   </si>
   <si>
-    <t>CONTEXTE DE BASE: Stable, croissance économique, population vieillissante</t>
-  </si>
-  <si>
     <t>PONDÉRATION (Variable selon contexte)</t>
+  </si>
+  <si>
+    <t>FITNESS :</t>
+  </si>
+  <si>
+    <t>CONTEXTE DE BASE: Stable, croissance économique, population vieillissante, taille 1000 individus</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Score pondéré</t>
+  </si>
+  <si>
+    <t>Apport positif</t>
+  </si>
+  <si>
+    <t>Total (avec coût)</t>
+  </si>
+  <si>
+    <t>Fa</t>
   </si>
 </sst>
 </file>
@@ -291,7 +309,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,6 +352,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -347,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -371,58 +395,73 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -740,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7D3F53-E2D2-416E-AD93-0175C9D788F7}">
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,23 +796,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
     </row>
     <row r="2" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -819,473 +858,473 @@
       <c r="A3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <v>0</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12" t="s">
+      <c r="E4" s="11"/>
+      <c r="F4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12" t="s">
+      <c r="H4" s="11"/>
+      <c r="I4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="12"/>
+      <c r="K4" s="11"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12" t="s">
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="12"/>
+      <c r="K5" s="11"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="12">
         <v>0.3</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12">
-        <v>1</v>
-      </c>
-      <c r="F6" s="12" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11">
+        <v>1</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12" t="s">
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="12"/>
+      <c r="K6" s="11"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="12">
         <v>0.2</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="12">
         <v>0.05</v>
       </c>
-      <c r="C8" s="12">
-        <v>1</v>
-      </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12" t="s">
+      <c r="C8" s="11">
+        <v>1</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="K9" s="12"/>
+      <c r="K9" s="11"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="K10" s="12"/>
+      <c r="K10" s="11"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="12" t="s">
+      <c r="B11" s="12"/>
+      <c r="C11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12" t="s">
+      <c r="D11" s="11"/>
+      <c r="E11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12" t="s">
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="12"/>
+      <c r="K11" s="11"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="12">
         <v>0.15</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12" t="s">
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12" t="s">
+      <c r="H12" s="11"/>
+      <c r="I12" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="J12" s="14" t="s">
+      <c r="J12" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="12"/>
+      <c r="K12" s="11"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="11"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12" t="s">
+      <c r="B14" s="12"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12" t="s">
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="12" t="s">
+      <c r="J14" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="K14" s="12"/>
+      <c r="K14" s="11"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="12">
         <v>0.1</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12" t="s">
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12" t="s">
+      <c r="H15" s="11"/>
+      <c r="I15" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="J15" s="12" t="s">
+      <c r="J15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="12"/>
+      <c r="K15" s="11"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12" t="s">
+      <c r="B16" s="12"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12" t="s">
+      <c r="H16" s="11"/>
+      <c r="I16" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12" t="s">
+      <c r="B17" s="12"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12" t="s">
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="J17" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="K17" s="12"/>
+      <c r="K17" s="11"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12" t="s">
+      <c r="B18" s="12"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12" t="s">
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="12" t="s">
+      <c r="I18" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="12" t="s">
+      <c r="J18" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="K18" s="12"/>
+      <c r="K18" s="11"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="13">
+      <c r="B19" s="12">
         <v>0</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="12">
-        <v>1</v>
-      </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
+      <c r="D19" s="11">
+        <v>1</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="14">
         <f>SUM(B4:B19)</f>
         <v>0.8</v>
       </c>
-      <c r="C20" s="16">
-        <v>1</v>
-      </c>
-      <c r="D20" s="16">
-        <v>1</v>
-      </c>
-      <c r="E20" s="16">
-        <v>1</v>
-      </c>
-      <c r="F20" s="16">
-        <v>1</v>
-      </c>
-      <c r="G20" s="16">
-        <v>1</v>
-      </c>
-      <c r="H20" s="16">
-        <v>1</v>
-      </c>
-      <c r="I20" s="16">
-        <v>1</v>
-      </c>
-      <c r="J20" s="16">
-        <v>1</v>
-      </c>
-      <c r="K20" s="12"/>
+      <c r="C20" s="15">
+        <v>1</v>
+      </c>
+      <c r="D20" s="15">
+        <v>1</v>
+      </c>
+      <c r="E20" s="15">
+        <v>1</v>
+      </c>
+      <c r="F20" s="15">
+        <v>1</v>
+      </c>
+      <c r="G20" s="15">
+        <v>1</v>
+      </c>
+      <c r="H20" s="15">
+        <v>1</v>
+      </c>
+      <c r="I20" s="15">
+        <v>1</v>
+      </c>
+      <c r="J20" s="15">
+        <v>1</v>
+      </c>
+      <c r="K20" s="11"/>
     </row>
     <row r="21" spans="1:16" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11" t="s">
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11">
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="1:16" s="19" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+    </row>
+    <row r="25" spans="1:16" s="18" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
@@ -1293,7 +1332,7 @@
       <c r="P25" s="5"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="9" t="s">
         <v>51</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1310,26 +1349,26 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="20">
+      <c r="B28" s="19">
         <v>0.5</v>
       </c>
-      <c r="C28" s="20">
+      <c r="C28" s="19">
         <v>0</v>
       </c>
-      <c r="D28" s="20">
+      <c r="D28" s="19">
         <v>0</v>
       </c>
-      <c r="E28" s="20">
+      <c r="E28" s="19">
         <v>0.8</v>
       </c>
     </row>
@@ -1337,16 +1376,16 @@
       <c r="A29" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="20">
+      <c r="B29" s="19">
         <v>0.375</v>
       </c>
-      <c r="C29" s="20">
+      <c r="C29" s="19">
         <v>0.15</v>
       </c>
-      <c r="D29" s="20">
+      <c r="D29" s="19">
         <v>0.35</v>
       </c>
-      <c r="E29" s="20">
+      <c r="E29" s="19">
         <v>0.125</v>
       </c>
     </row>
@@ -1354,16 +1393,16 @@
       <c r="A30" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="20">
+      <c r="B30" s="19">
         <v>0.1</v>
       </c>
-      <c r="C30" s="20">
+      <c r="C30" s="19">
         <v>0.6</v>
       </c>
-      <c r="D30" s="20">
+      <c r="D30" s="19">
         <v>0</v>
       </c>
-      <c r="E30" s="20">
+      <c r="E30" s="19">
         <v>0.05</v>
       </c>
     </row>
@@ -1371,25 +1410,25 @@
       <c r="A31" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="20">
+      <c r="B31" s="19">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C31" s="20">
+      <c r="C31" s="19">
         <v>0.25</v>
       </c>
-      <c r="D31" s="20">
+      <c r="D31" s="19">
         <v>0.65</v>
       </c>
-      <c r="E31" s="20">
+      <c r="E31" s="19">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
@@ -1402,110 +1441,298 @@
       <c r="O32" s="7"/>
       <c r="P32" s="7"/>
     </row>
-    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="22">
+      <c r="B33" s="21">
         <f>SUM(B28:B31)</f>
         <v>1</v>
       </c>
-      <c r="C33" s="22">
+      <c r="C33" s="21">
         <f>SUM(C28:C31)</f>
         <v>1</v>
       </c>
-      <c r="D33" s="22">
+      <c r="D33" s="21">
         <f>SUM(D28:D31)</f>
         <v>1</v>
       </c>
-      <c r="E33" s="22">
+      <c r="E33" s="21">
         <f>SUM(E28:E31)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="24" t="s">
+    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="22">
+        <v>0.1</v>
+      </c>
+      <c r="C34" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="D34" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="E34" s="22">
+        <v>0.4</v>
+      </c>
+      <c r="F34" s="20">
+        <f>SUM(B34:E34)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <f>SUM(A40:A43)</f>
+        <v>4</v>
+      </c>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>1</v>
+      </c>
+      <c r="B40" s="30">
+        <f>PRODUCT(B28,$A40)</f>
+        <v>0.5</v>
+      </c>
+      <c r="C40" s="30">
+        <f t="shared" ref="C40:E40" si="0">PRODUCT(C28,$A40)</f>
+        <v>0</v>
+      </c>
+      <c r="D40" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E40" s="30">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="F40" s="28">
+        <f>SUM(C40:E40)</f>
+        <v>0.8</v>
+      </c>
+      <c r="G40" s="3">
+        <f>F40-B40</f>
+        <v>0.30000000000000004</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>1</v>
+      </c>
+      <c r="B41" s="8">
+        <f>PRODUCT(B29,$A41)</f>
+        <v>0.375</v>
+      </c>
+      <c r="C41" s="8">
+        <f t="shared" ref="C41:E43" si="1">PRODUCT(C29,$A41)</f>
+        <v>0.15</v>
+      </c>
+      <c r="D41" s="8">
+        <f t="shared" si="1"/>
+        <v>0.35</v>
+      </c>
+      <c r="E41" s="8">
+        <f t="shared" si="1"/>
+        <v>0.125</v>
+      </c>
+      <c r="F41" s="28">
+        <f t="shared" ref="F41:F44" si="2">SUM(C41:E41)</f>
+        <v>0.625</v>
+      </c>
+      <c r="G41" s="8">
+        <f t="shared" ref="G41:G44" si="3">F41-B41</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>1</v>
+      </c>
+      <c r="B42" s="8">
+        <f>PRODUCT(B30,$A42)</f>
+        <v>0.1</v>
+      </c>
+      <c r="C42" s="8">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="D42" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E42" s="8">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="F42" s="28">
+        <f t="shared" si="2"/>
+        <v>0.65</v>
+      </c>
+      <c r="G42" s="8">
+        <f t="shared" si="3"/>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>1</v>
+      </c>
+      <c r="B43" s="8">
+        <f>PRODUCT(B31,$A43)</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C43" s="8">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="D43" s="8">
+        <f t="shared" si="1"/>
+        <v>0.65</v>
+      </c>
+      <c r="E43" s="8">
+        <f t="shared" si="1"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F43" s="28">
+        <f t="shared" si="2"/>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="G43" s="8">
+        <f t="shared" si="3"/>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B44" s="8">
+        <f>SUM(B40:B43)</f>
+        <v>1</v>
+      </c>
+      <c r="C44" s="8">
+        <f t="shared" ref="C44:E44" si="4">SUM(C40:C43)</f>
+        <v>1</v>
+      </c>
+      <c r="D44" s="8">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E44" s="8">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F44" s="28"/>
+      <c r="G44" s="8"/>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="27">
+        <v>1</v>
+      </c>
+      <c r="C45" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="D45" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="E45" s="22">
+        <v>0.4</v>
+      </c>
+      <c r="F45" s="28"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" s="8">
+        <f>PRODUCT(B44:B45)</f>
+        <v>1</v>
+      </c>
+      <c r="C46" s="8">
+        <f t="shared" ref="C46:E46" si="5">PRODUCT(C44:C45)</f>
+        <v>0.3</v>
+      </c>
+      <c r="D46" s="8">
+        <f t="shared" si="5"/>
+        <v>0.3</v>
+      </c>
+      <c r="E46" s="8">
+        <f t="shared" si="5"/>
+        <v>0.4</v>
+      </c>
+      <c r="F46" s="28"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="23">
-        <v>0.1</v>
-      </c>
-      <c r="C34" s="23">
-        <v>0.2</v>
-      </c>
-      <c r="D34" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="E34" s="23">
-        <v>0.4</v>
-      </c>
-      <c r="F34" s="21">
-        <f>SUM(B34:E34)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C49" s="3">
+        <f>SUM(C46:E46)-B46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
     </row>
   </sheetData>
@@ -1521,6 +1748,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010006B233B9B3A5024C99847B1D0443027F" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="39a3a9a18fc0038d1c425abb13176a98">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d59a1f78-4cdc-402c-b8a0-58bfb80633d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="635a148d9eedb07babeb6ca05c95a7d9" ns3:_="">
     <xsd:import namespace="d59a1f78-4cdc-402c-b8a0-58bfb80633d0"/>
@@ -1652,22 +1894,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C4C12EB-A87C-4B65-A0A2-3CFB630D4604}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d59a1f78-4cdc-402c-b8a0-58bfb80633d0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F3EA1CF-A27A-4CFA-9674-6A86EB7CE3B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D72B6365-5724-4DCC-8EE2-F84342C5EBFF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1683,28 +1934,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F3EA1CF-A27A-4CFA-9674-6A86EB7CE3B7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C4C12EB-A87C-4B65-A0A2-3CFB630D4604}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="d59a1f78-4cdc-402c-b8a0-58bfb80633d0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
work work happy community on model
</commit_message>
<xml_diff>
--- a/problem 3 - concept/jobs.xlsx
+++ b/problem 3 - concept/jobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deric\Desktop\ai-genetic\ai-projet2-genetic\problem 3 - concept\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A5E260-3EDB-48CF-AE71-DB1F38D7ABA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C270AA7D-58AB-4AA0-A383-886A2DA1CD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10920" yWindow="1080" windowWidth="28785" windowHeight="14505" xr2:uid="{2134C11B-C8CC-4877-9366-45380615B26B}"/>
+    <workbookView xWindow="7575" yWindow="1290" windowWidth="28785" windowHeight="14505" xr2:uid="{2134C11B-C8CC-4877-9366-45380615B26B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -442,6 +442,18 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -450,18 +462,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -779,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7D3F53-E2D2-416E-AD93-0175C9D788F7}">
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,23 +796,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
     </row>
     <row r="2" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1278,53 +1278,53 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
     </row>
     <row r="25" spans="1:16" s="18" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="30"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
@@ -1498,21 +1498,21 @@
     </row>
     <row r="38" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <f>SUM(A40:A43)</f>
-        <v>4</v>
-      </c>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
+        <v>19</v>
+      </c>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
       <c r="F39" s="8" t="s">
         <v>66</v>
       </c>
@@ -1522,31 +1522,31 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
-        <v>1</v>
-      </c>
-      <c r="B40" s="30">
+        <v>2</v>
+      </c>
+      <c r="B40" s="27">
         <f>PRODUCT(B28,$A40)</f>
-        <v>0.5</v>
-      </c>
-      <c r="C40" s="30">
+        <v>1</v>
+      </c>
+      <c r="C40" s="27">
         <f t="shared" ref="C40:E40" si="0">PRODUCT(C28,$A40)</f>
         <v>0</v>
       </c>
-      <c r="D40" s="30">
+      <c r="D40" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E40" s="30">
+      <c r="E40" s="27">
         <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="F40" s="28">
+        <v>1.6</v>
+      </c>
+      <c r="F40" s="25">
         <f>SUM(C40:E40)</f>
-        <v>0.8</v>
+        <v>1.6</v>
       </c>
       <c r="G40" s="3">
         <f>F40-B40</f>
-        <v>0.30000000000000004</v>
+        <v>0.60000000000000009</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1569,26 +1569,26 @@
         <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
-      <c r="F41" s="28">
-        <f t="shared" ref="F41:F44" si="2">SUM(C41:E41)</f>
+      <c r="F41" s="25">
+        <f t="shared" ref="F41:F43" si="2">SUM(C41:E41)</f>
         <v>0.625</v>
       </c>
       <c r="G41" s="8">
-        <f t="shared" ref="G41:G44" si="3">F41-B41</f>
+        <f t="shared" ref="G41:G43" si="3">F41-B41</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B42" s="8">
         <f>PRODUCT(B30,$A42)</f>
-        <v>0.1</v>
+        <v>1.5</v>
       </c>
       <c r="C42" s="8">
         <f t="shared" si="1"/>
-        <v>0.6</v>
+        <v>9</v>
       </c>
       <c r="D42" s="8">
         <f t="shared" si="1"/>
@@ -1596,15 +1596,15 @@
       </c>
       <c r="E42" s="8">
         <f t="shared" si="1"/>
-        <v>0.05</v>
-      </c>
-      <c r="F42" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="F42" s="25">
         <f t="shared" si="2"/>
-        <v>0.65</v>
+        <v>9.75</v>
       </c>
       <c r="G42" s="8">
         <f t="shared" si="3"/>
-        <v>0.55000000000000004</v>
+        <v>8.25</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1627,7 +1627,7 @@
         <f t="shared" si="1"/>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F43" s="28">
+      <c r="F43" s="25">
         <f t="shared" si="2"/>
         <v>0.92500000000000004</v>
       </c>
@@ -1642,11 +1642,11 @@
       </c>
       <c r="B44" s="8">
         <f>SUM(B40:B43)</f>
-        <v>1</v>
+        <v>2.9</v>
       </c>
       <c r="C44" s="8">
         <f t="shared" ref="C44:E44" si="4">SUM(C40:C43)</f>
-        <v>1</v>
+        <v>9.4</v>
       </c>
       <c r="D44" s="8">
         <f t="shared" si="4"/>
@@ -1654,26 +1654,26 @@
       </c>
       <c r="E44" s="8">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="F44" s="28"/>
+        <v>2.5</v>
+      </c>
+      <c r="F44" s="25"/>
       <c r="G44" s="8"/>
     </row>
     <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
-      <c r="B45" s="27">
+      <c r="B45" s="24">
         <v>1</v>
       </c>
       <c r="C45" s="22">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="D45" s="22">
         <v>0.3</v>
       </c>
       <c r="E45" s="22">
-        <v>0.4</v>
-      </c>
-      <c r="F45" s="28"/>
+        <v>0.2</v>
+      </c>
+      <c r="F45" s="25"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
@@ -1681,11 +1681,11 @@
       </c>
       <c r="B46" s="8">
         <f>PRODUCT(B44:B45)</f>
-        <v>1</v>
+        <v>2.9</v>
       </c>
       <c r="C46" s="8">
         <f t="shared" ref="C46:E46" si="5">PRODUCT(C44:C45)</f>
-        <v>0.3</v>
+        <v>4.7</v>
       </c>
       <c r="D46" s="8">
         <f t="shared" si="5"/>
@@ -1693,9 +1693,9 @@
       </c>
       <c r="E46" s="8">
         <f t="shared" si="5"/>
-        <v>0.4</v>
-      </c>
-      <c r="F46" s="28"/>
+        <v>0.5</v>
+      </c>
+      <c r="F46" s="25"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
@@ -1715,7 +1715,7 @@
       </c>
       <c r="C49" s="3">
         <f>SUM(C46:E46)-B46</f>
-        <v>0</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1748,21 +1748,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010006B233B9B3A5024C99847B1D0443027F" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="39a3a9a18fc0038d1c425abb13176a98">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d59a1f78-4cdc-402c-b8a0-58bfb80633d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="635a148d9eedb07babeb6ca05c95a7d9" ns3:_="">
     <xsd:import namespace="d59a1f78-4cdc-402c-b8a0-58bfb80633d0"/>
@@ -1894,31 +1879,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C4C12EB-A87C-4B65-A0A2-3CFB630D4604}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="d59a1f78-4cdc-402c-b8a0-58bfb80633d0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F3EA1CF-A27A-4CFA-9674-6A86EB7CE3B7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D72B6365-5724-4DCC-8EE2-F84342C5EBFF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1934,4 +1910,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F3EA1CF-A27A-4CFA-9674-6A86EB7CE3B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C4C12EB-A87C-4B65-A0A2-3CFB630D4604}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d59a1f78-4cdc-402c-b8a0-58bfb80633d0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
working on prob 3 with a test main
</commit_message>
<xml_diff>
--- a/problem 3 - concept/jobs.xlsx
+++ b/problem 3 - concept/jobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deric\Desktop\ai-genetic\ai-projet2-genetic\problem 3 - concept\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C270AA7D-58AB-4AA0-A383-886A2DA1CD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D374F0A0-9974-4FE1-97DB-D994D5826945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7575" yWindow="1290" windowWidth="28785" windowHeight="14505" xr2:uid="{2134C11B-C8CC-4877-9366-45380615B26B}"/>
+    <workbookView xWindow="15" yWindow="1245" windowWidth="28785" windowHeight="14505" xr2:uid="{2134C11B-C8CC-4877-9366-45380615B26B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -779,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7D3F53-E2D2-416E-AD93-0175C9D788F7}">
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1665,13 +1665,13 @@
         <v>1</v>
       </c>
       <c r="C45" s="22">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D45" s="22">
         <v>0.3</v>
       </c>
       <c r="E45" s="22">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="F45" s="25"/>
     </row>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="C46" s="8">
         <f t="shared" ref="C46:E46" si="5">PRODUCT(C44:C45)</f>
-        <v>4.7</v>
+        <v>2.82</v>
       </c>
       <c r="D46" s="8">
         <f t="shared" si="5"/>
@@ -1693,7 +1693,7 @@
       </c>
       <c r="E46" s="8">
         <f t="shared" si="5"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F46" s="25"/>
     </row>
@@ -1715,7 +1715,7 @@
       </c>
       <c r="C49" s="3">
         <f>SUM(C46:E46)-B46</f>
-        <v>2.6</v>
+        <v>1.2199999999999993</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1748,6 +1748,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010006B233B9B3A5024C99847B1D0443027F" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="39a3a9a18fc0038d1c425abb13176a98">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d59a1f78-4cdc-402c-b8a0-58bfb80633d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="635a148d9eedb07babeb6ca05c95a7d9" ns3:_="">
     <xsd:import namespace="d59a1f78-4cdc-402c-b8a0-58bfb80633d0"/>
@@ -1879,22 +1894,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C4C12EB-A87C-4B65-A0A2-3CFB630D4604}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d59a1f78-4cdc-402c-b8a0-58bfb80633d0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F3EA1CF-A27A-4CFA-9674-6A86EB7CE3B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D72B6365-5724-4DCC-8EE2-F84342C5EBFF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1910,28 +1934,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F3EA1CF-A27A-4CFA-9674-6A86EB7CE3B7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C4C12EB-A87C-4B65-A0A2-3CFB630D4604}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="d59a1f78-4cdc-402c-b8a0-58bfb80633d0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
model on right tracks for problem 3
</commit_message>
<xml_diff>
--- a/problem 3 - concept/jobs.xlsx
+++ b/problem 3 - concept/jobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deric\Desktop\ai-genetic\ai-projet2-genetic\problem 3 - concept\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D374F0A0-9974-4FE1-97DB-D994D5826945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9D91CA-7162-4F56-89A8-1AAE97DC1987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="1245" windowWidth="28785" windowHeight="14505" xr2:uid="{2134C11B-C8CC-4877-9366-45380615B26B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{2134C11B-C8CC-4877-9366-45380615B26B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -780,7 +780,7 @@
   <dimension ref="A1:P54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1508,7 +1508,7 @@
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <f>SUM(A40:A43)</f>
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C39" s="25"/>
       <c r="D39" s="25"/>
@@ -1522,11 +1522,11 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B40" s="27">
         <f>PRODUCT(B28,$A40)</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C40" s="27">
         <f t="shared" ref="C40:E40" si="0">PRODUCT(C28,$A40)</f>
@@ -1538,57 +1538,57 @@
       </c>
       <c r="E40" s="27">
         <f t="shared" si="0"/>
-        <v>1.6</v>
+        <v>2.4000000000000004</v>
       </c>
       <c r="F40" s="25">
         <f>SUM(C40:E40)</f>
-        <v>1.6</v>
+        <v>2.4000000000000004</v>
       </c>
       <c r="G40" s="3">
         <f>F40-B40</f>
-        <v>0.60000000000000009</v>
+        <v>0.90000000000000036</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B41" s="8">
         <f>PRODUCT(B29,$A41)</f>
-        <v>0.375</v>
+        <v>0.75</v>
       </c>
       <c r="C41" s="8">
         <f t="shared" ref="C41:E43" si="1">PRODUCT(C29,$A41)</f>
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="D41" s="8">
         <f t="shared" si="1"/>
-        <v>0.35</v>
+        <v>0.7</v>
       </c>
       <c r="E41" s="8">
         <f t="shared" si="1"/>
-        <v>0.125</v>
+        <v>0.25</v>
       </c>
       <c r="F41" s="25">
         <f t="shared" ref="F41:F43" si="2">SUM(C41:E41)</f>
-        <v>0.625</v>
+        <v>1.25</v>
       </c>
       <c r="G41" s="8">
         <f t="shared" ref="G41:G43" si="3">F41-B41</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B42" s="8">
         <f>PRODUCT(B30,$A42)</f>
-        <v>1.5</v>
+        <v>0.2</v>
       </c>
       <c r="C42" s="8">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>1.2</v>
       </c>
       <c r="D42" s="8">
         <f t="shared" si="1"/>
@@ -1596,44 +1596,44 @@
       </c>
       <c r="E42" s="8">
         <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>0.1</v>
       </c>
       <c r="F42" s="25">
         <f t="shared" si="2"/>
-        <v>9.75</v>
+        <v>1.3</v>
       </c>
       <c r="G42" s="8">
         <f t="shared" si="3"/>
-        <v>8.25</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B43" s="8">
         <f>PRODUCT(B31,$A43)</f>
-        <v>2.5000000000000001E-2</v>
+        <v>7.5000000000000011E-2</v>
       </c>
       <c r="C43" s="8">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="D43" s="8">
         <f t="shared" si="1"/>
-        <v>0.65</v>
+        <v>1.9500000000000002</v>
       </c>
       <c r="E43" s="8">
         <f t="shared" si="1"/>
-        <v>2.5000000000000001E-2</v>
+        <v>7.5000000000000011E-2</v>
       </c>
       <c r="F43" s="25">
         <f t="shared" si="2"/>
-        <v>0.92500000000000004</v>
+        <v>2.7750000000000004</v>
       </c>
       <c r="G43" s="8">
         <f t="shared" si="3"/>
-        <v>0.9</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1642,19 +1642,19 @@
       </c>
       <c r="B44" s="8">
         <f>SUM(B40:B43)</f>
-        <v>2.9</v>
+        <v>2.5250000000000004</v>
       </c>
       <c r="C44" s="8">
         <f t="shared" ref="C44:E44" si="4">SUM(C40:C43)</f>
-        <v>9.4</v>
+        <v>2.25</v>
       </c>
       <c r="D44" s="8">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2.6500000000000004</v>
       </c>
       <c r="E44" s="8">
         <f t="shared" si="4"/>
-        <v>2.5</v>
+        <v>2.8250000000000006</v>
       </c>
       <c r="F44" s="25"/>
       <c r="G44" s="8"/>
@@ -1681,19 +1681,19 @@
       </c>
       <c r="B46" s="8">
         <f>PRODUCT(B44:B45)</f>
-        <v>2.9</v>
+        <v>2.5250000000000004</v>
       </c>
       <c r="C46" s="8">
         <f t="shared" ref="C46:E46" si="5">PRODUCT(C44:C45)</f>
-        <v>2.82</v>
+        <v>0.67499999999999993</v>
       </c>
       <c r="D46" s="8">
         <f t="shared" si="5"/>
-        <v>0.3</v>
+        <v>0.79500000000000004</v>
       </c>
       <c r="E46" s="8">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>1.1300000000000003</v>
       </c>
       <c r="F46" s="25"/>
     </row>
@@ -1715,7 +1715,7 @@
       </c>
       <c r="C49" s="3">
         <f>SUM(C46:E46)-B46</f>
-        <v>1.2199999999999993</v>
+        <v>7.5000000000000178E-2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1748,21 +1748,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010006B233B9B3A5024C99847B1D0443027F" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="39a3a9a18fc0038d1c425abb13176a98">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d59a1f78-4cdc-402c-b8a0-58bfb80633d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="635a148d9eedb07babeb6ca05c95a7d9" ns3:_="">
     <xsd:import namespace="d59a1f78-4cdc-402c-b8a0-58bfb80633d0"/>
@@ -1894,31 +1879,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C4C12EB-A87C-4B65-A0A2-3CFB630D4604}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="d59a1f78-4cdc-402c-b8a0-58bfb80633d0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F3EA1CF-A27A-4CFA-9674-6A86EB7CE3B7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D72B6365-5724-4DCC-8EE2-F84342C5EBFF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1934,4 +1910,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F3EA1CF-A27A-4CFA-9674-6A86EB7CE3B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C4C12EB-A87C-4B65-A0A2-3CFB630D4604}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d59a1f78-4cdc-402c-b8a0-58bfb80633d0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
working fitness with exponential function
</commit_message>
<xml_diff>
--- a/problem 3 - concept/jobs.xlsx
+++ b/problem 3 - concept/jobs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deric\Desktop\ai-genetic\ai-projet2-genetic\problem 3 - concept\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9D91CA-7162-4F56-89A8-1AAE97DC1987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED3EED9-4CBB-4D0A-82CB-82C64F1D5FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{2134C11B-C8CC-4877-9366-45380615B26B}"/>
   </bookViews>
@@ -223,9 +223,6 @@
     <t>PONDÉRATION (Variable selon contexte)</t>
   </si>
   <si>
-    <t>FITNESS :</t>
-  </si>
-  <si>
     <t>CONTEXTE DE BASE: Stable, croissance économique, population vieillissante, taille 1000 individus</t>
   </si>
   <si>
@@ -241,7 +238,10 @@
     <t>Total (avec coût)</t>
   </si>
   <si>
-    <t>Fa</t>
+    <t>y = a^(1/x)</t>
+  </si>
+  <si>
+    <t>16 jobs</t>
   </si>
 </sst>
 </file>
@@ -371,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -453,6 +453,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -779,14 +782,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7D3F53-E2D2-416E-AD93-0175C9D788F7}">
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="56.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="29.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="25.5703125" style="3" customWidth="1"/>
@@ -796,23 +799,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
     </row>
     <row r="2" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1278,53 +1281,55 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
     </row>
     <row r="25" spans="1:16" s="18" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="30"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="30"/>
+      <c r="A25" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
@@ -1360,7 +1365,7 @@
         <v>52</v>
       </c>
       <c r="B28" s="19">
-        <v>0.5</v>
+        <v>0.12</v>
       </c>
       <c r="C28" s="19">
         <v>0</v>
@@ -1369,7 +1374,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="19">
-        <v>0.8</v>
+        <v>0.77500000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -1377,16 +1382,16 @@
         <v>53</v>
       </c>
       <c r="B29" s="19">
-        <v>0.375</v>
+        <v>0.1</v>
       </c>
       <c r="C29" s="19">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="D29" s="19">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="E29" s="19">
-        <v>0.125</v>
+        <v>0.14749999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -1394,7 +1399,7 @@
         <v>54</v>
       </c>
       <c r="B30" s="19">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="C30" s="19">
         <v>0.6</v>
@@ -1403,7 +1408,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="19">
-        <v>0.05</v>
+        <v>7.4999999999999997E-3</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -1411,16 +1416,16 @@
         <v>55</v>
       </c>
       <c r="B31" s="19">
-        <v>2.5000000000000001E-2</v>
+        <v>0.06</v>
       </c>
       <c r="C31" s="19">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="D31" s="19">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="E31" s="19">
-        <v>2.5000000000000001E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -1447,7 +1452,7 @@
       </c>
       <c r="B33" s="21">
         <f>SUM(B28:B31)</f>
-        <v>1</v>
+        <v>0.36</v>
       </c>
       <c r="C33" s="21">
         <f>SUM(C28:C31)</f>
@@ -1490,7 +1495,7 @@
     </row>
     <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1508,25 +1513,25 @@
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <f>SUM(A40:A43)</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C39" s="25"/>
       <c r="D39" s="25"/>
       <c r="E39" s="25"/>
       <c r="F39" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G39" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="G39" s="8" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B40" s="27">
-        <f>PRODUCT(B28,$A40)</f>
-        <v>1.5</v>
+        <f>B28^(1/A40)</f>
+        <v>0.12</v>
       </c>
       <c r="C40" s="27">
         <f t="shared" ref="C40:E40" si="0">PRODUCT(C28,$A40)</f>
@@ -1538,57 +1543,57 @@
       </c>
       <c r="E40" s="27">
         <f t="shared" si="0"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="F40" s="25">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="F40" s="28">
         <f>SUM(C40:E40)</f>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="G40" s="3">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="G40" s="28">
         <f>F40-B40</f>
-        <v>0.90000000000000036</v>
+        <v>0.65500000000000003</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
-        <v>2</v>
-      </c>
-      <c r="B41" s="8">
-        <f>PRODUCT(B29,$A41)</f>
-        <v>0.75</v>
+        <v>3</v>
+      </c>
+      <c r="B41" s="27">
+        <f>B29^(1/A41)</f>
+        <v>0.46415888336127797</v>
       </c>
       <c r="C41" s="8">
         <f t="shared" ref="C41:E43" si="1">PRODUCT(C29,$A41)</f>
-        <v>0.3</v>
+        <v>0.75</v>
       </c>
       <c r="D41" s="8">
         <f t="shared" si="1"/>
-        <v>0.7</v>
+        <v>1.2000000000000002</v>
       </c>
       <c r="E41" s="8">
         <f t="shared" si="1"/>
-        <v>0.25</v>
-      </c>
-      <c r="F41" s="25">
-        <f t="shared" ref="F41:F43" si="2">SUM(C41:E41)</f>
-        <v>1.25</v>
-      </c>
-      <c r="G41" s="8">
-        <f t="shared" ref="G41:G43" si="3">F41-B41</f>
-        <v>0.5</v>
+        <v>0.4425</v>
+      </c>
+      <c r="F41" s="28">
+        <f>SUM(C41:E41)</f>
+        <v>2.3925000000000001</v>
+      </c>
+      <c r="G41" s="28">
+        <f>F41-B41</f>
+        <v>1.9283411166387221</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <v>2</v>
-      </c>
-      <c r="B42" s="8">
-        <f>PRODUCT(B30,$A42)</f>
-        <v>0.2</v>
+        <v>1</v>
+      </c>
+      <c r="B42" s="27">
+        <f>B30^(1/A42)</f>
+        <v>0.08</v>
       </c>
       <c r="C42" s="8">
         <f t="shared" si="1"/>
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="D42" s="8">
         <f t="shared" si="1"/>
@@ -1596,68 +1601,67 @@
       </c>
       <c r="E42" s="8">
         <f t="shared" si="1"/>
-        <v>0.1</v>
-      </c>
-      <c r="F42" s="25">
-        <f t="shared" si="2"/>
-        <v>1.3</v>
-      </c>
-      <c r="G42" s="8">
-        <f t="shared" si="3"/>
-        <v>1.1000000000000001</v>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="F42" s="28">
+        <f>SUM(C42:E42)</f>
+        <v>0.60749999999999993</v>
+      </c>
+      <c r="G42" s="28">
+        <f>F42-B42</f>
+        <v>0.52749999999999997</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
-        <v>3</v>
-      </c>
-      <c r="B43" s="8">
-        <f>PRODUCT(B31,$A43)</f>
-        <v>7.5000000000000011E-2</v>
+        <v>2</v>
+      </c>
+      <c r="B43" s="27">
+        <f>B31^(1/A43)</f>
+        <v>0.2449489742783178</v>
       </c>
       <c r="C43" s="8">
         <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>0.3</v>
       </c>
       <c r="D43" s="8">
-        <f t="shared" si="1"/>
-        <v>1.9500000000000002</v>
+        <f>PRODUCT(D31,$A43)</f>
+        <v>1.2</v>
       </c>
       <c r="E43" s="8">
         <f t="shared" si="1"/>
-        <v>7.5000000000000011E-2</v>
-      </c>
-      <c r="F43" s="25">
-        <f t="shared" si="2"/>
-        <v>2.7750000000000004</v>
-      </c>
-      <c r="G43" s="8">
-        <f t="shared" si="3"/>
-        <v>2.7</v>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F43" s="28">
+        <f>SUM(C43:E43)</f>
+        <v>1.6400000000000001</v>
+      </c>
+      <c r="G43" s="28">
+        <f>F43-B43</f>
+        <v>1.3950510257216824</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B44" s="8">
         <f>SUM(B40:B43)</f>
-        <v>2.5250000000000004</v>
+        <v>0.90910785763959567</v>
       </c>
       <c r="C44" s="8">
-        <f t="shared" ref="C44:E44" si="4">SUM(C40:C43)</f>
-        <v>2.25</v>
+        <f t="shared" ref="C44:E44" si="2">SUM(C40:C43)</f>
+        <v>1.6500000000000001</v>
       </c>
       <c r="D44" s="8">
-        <f t="shared" si="4"/>
-        <v>2.6500000000000004</v>
+        <f t="shared" si="2"/>
+        <v>2.4000000000000004</v>
       </c>
       <c r="E44" s="8">
-        <f t="shared" si="4"/>
-        <v>2.8250000000000006</v>
+        <f t="shared" si="2"/>
+        <v>1.3650000000000002</v>
       </c>
       <c r="F44" s="25"/>
-      <c r="G44" s="8"/>
     </row>
     <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
@@ -1677,23 +1681,23 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B46" s="8">
         <f>PRODUCT(B44:B45)</f>
-        <v>2.5250000000000004</v>
+        <v>0.90910785763959567</v>
       </c>
       <c r="C46" s="8">
-        <f t="shared" ref="C46:E46" si="5">PRODUCT(C44:C45)</f>
-        <v>0.67499999999999993</v>
+        <f t="shared" ref="C46:E46" si="3">PRODUCT(C44:C45)</f>
+        <v>0.495</v>
       </c>
       <c r="D46" s="8">
-        <f t="shared" si="5"/>
-        <v>0.79500000000000004</v>
+        <f t="shared" si="3"/>
+        <v>0.72000000000000008</v>
       </c>
       <c r="E46" s="8">
-        <f t="shared" si="5"/>
-        <v>1.1300000000000003</v>
+        <f t="shared" si="3"/>
+        <v>0.54600000000000015</v>
       </c>
       <c r="F46" s="25"/>
     </row>
@@ -1708,31 +1712,26 @@
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
-      <c r="B49" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C49" s="3">
-        <f>SUM(C46:E46)-B46</f>
-        <v>7.5000000000000178E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="8"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
     </row>
   </sheetData>
@@ -1748,6 +1747,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010006B233B9B3A5024C99847B1D0443027F" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="39a3a9a18fc0038d1c425abb13176a98">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d59a1f78-4cdc-402c-b8a0-58bfb80633d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="635a148d9eedb07babeb6ca05c95a7d9" ns3:_="">
     <xsd:import namespace="d59a1f78-4cdc-402c-b8a0-58bfb80633d0"/>
@@ -1879,22 +1893,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C4C12EB-A87C-4B65-A0A2-3CFB630D4604}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d59a1f78-4cdc-402c-b8a0-58bfb80633d0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F3EA1CF-A27A-4CFA-9674-6A86EB7CE3B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D72B6365-5724-4DCC-8EE2-F84342C5EBFF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1910,28 +1933,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F3EA1CF-A27A-4CFA-9674-6A86EB7CE3B7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C4C12EB-A87C-4B65-A0A2-3CFB630D4604}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="d59a1f78-4cdc-402c-b8a0-58bfb80633d0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
jobs value in code
</commit_message>
<xml_diff>
--- a/problem 3 - concept/jobs.xlsx
+++ b/problem 3 - concept/jobs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deric\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deric\Desktop\ai-genetic\ai-projet2-genetic\problem 3 - concept\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8F76B2-EC32-443E-9068-D2716740921C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12929D35-8249-4AA1-85DF-3536C0B512D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{2134C11B-C8CC-4877-9366-45380615B26B}"/>
+    <workbookView xWindow="14775" yWindow="2325" windowWidth="23970" windowHeight="14505" xr2:uid="{2134C11B-C8CC-4877-9366-45380615B26B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -219,9 +219,6 @@
     <t xml:space="preserve">Ex : En temps de paix et de croissance économique, on se soucie moins d'avoir un gros Community Cost, En temps de guerre, c'est le contraire </t>
   </si>
   <si>
-    <t>Spiritual Enforcer[8]</t>
-  </si>
-  <si>
     <t>TOTAL PAR JOB</t>
   </si>
   <si>
@@ -229,6 +226,9 @@
   </si>
   <si>
     <t>Emergency[13]</t>
+  </si>
+  <si>
+    <t>Spiritual Leader[8]</t>
   </si>
 </sst>
 </file>
@@ -852,15 +852,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7D3F53-E2D2-416E-AD93-0175C9D788F7}">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="3" customWidth="1"/>
     <col min="4" max="4" width="29.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="22" style="3" customWidth="1"/>
     <col min="6" max="7" width="23.5703125" style="3" customWidth="1"/>
@@ -1442,7 +1442,7 @@
         <v>8</v>
       </c>
       <c r="K26" s="35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -1451,7 +1451,7 @@
       </c>
       <c r="B27" s="32">
         <f>K27/K43</f>
-        <v>0.10625</v>
+        <v>0.10312499999999999</v>
       </c>
       <c r="C27" s="32">
         <v>0.05</v>
@@ -1472,14 +1472,14 @@
         <v>0</v>
       </c>
       <c r="I27" s="32">
-        <v>0.1</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="J27" s="32">
         <v>0.1</v>
       </c>
       <c r="K27" s="35">
         <f>SUM(C27:J27)</f>
-        <v>0.85</v>
+        <v>0.82499999999999996</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -1488,7 +1488,7 @@
       </c>
       <c r="B28" s="32">
         <f>K28/K43</f>
-        <v>7.7500000000000013E-2</v>
+        <v>8.3750000000000005E-2</v>
       </c>
       <c r="C28" s="32">
         <v>0.15</v>
@@ -1500,7 +1500,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F28" s="32">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="G28" s="32">
         <v>0.1</v>
@@ -1516,7 +1516,7 @@
       </c>
       <c r="K28" s="35">
         <f>SUM(C28:J28)</f>
-        <v>0.62000000000000011</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -1641,7 +1641,7 @@
       </c>
       <c r="B32" s="32">
         <f>K32/K43</f>
-        <v>3.7500000000000006E-2</v>
+        <v>3.7687499999999999E-2</v>
       </c>
       <c r="C32" s="32">
         <v>0.05</v>
@@ -1650,7 +1650,7 @@
         <v>0.1</v>
       </c>
       <c r="E32" s="32">
-        <v>0</v>
+        <v>1.5E-3</v>
       </c>
       <c r="F32" s="32">
         <v>0</v>
@@ -1669,7 +1669,7 @@
       </c>
       <c r="K32" s="35">
         <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
+        <v>0.30149999999999999</v>
       </c>
       <c r="L32" s="25"/>
       <c r="M32" s="25"/>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="B34" s="32">
         <f>K34/K43</f>
-        <v>5.6250000000000001E-2</v>
+        <v>5.3125000000000006E-2</v>
       </c>
       <c r="C34" s="32">
         <v>0</v>
@@ -1746,14 +1746,14 @@
         <v>0</v>
       </c>
       <c r="I34" s="32">
-        <v>0</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="J34" s="32">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="K34" s="35">
         <f t="shared" si="0"/>
-        <v>0.45</v>
+        <v>0.42500000000000004</v>
       </c>
       <c r="L34" s="25"/>
       <c r="M34" s="25"/>
@@ -1763,11 +1763,11 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B35" s="32">
         <f>K35/K43</f>
-        <v>7.5000000000000011E-2</v>
+        <v>7.5625000000000012E-2</v>
       </c>
       <c r="C35" s="32">
         <v>0</v>
@@ -1788,14 +1788,14 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="I35" s="32">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="J35" s="32">
         <v>0</v>
       </c>
       <c r="K35" s="35">
         <f t="shared" si="0"/>
-        <v>0.60000000000000009</v>
+        <v>0.60500000000000009</v>
       </c>
       <c r="L35" s="25"/>
       <c r="M35" s="25"/>
@@ -1809,7 +1809,7 @@
       </c>
       <c r="B36" s="32">
         <f>K36/K43</f>
-        <v>3.4375000000000003E-2</v>
+        <v>2.75E-2</v>
       </c>
       <c r="C36" s="32">
         <v>0</v>
@@ -1821,7 +1821,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="32">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G36" s="32">
         <v>0</v>
@@ -1830,14 +1830,14 @@
         <v>0</v>
       </c>
       <c r="I36" s="32">
-        <v>0.125</v>
+        <v>0.12</v>
       </c>
       <c r="J36" s="32">
         <v>0</v>
       </c>
       <c r="K36" s="35">
         <f t="shared" si="0"/>
-        <v>0.27500000000000002</v>
+        <v>0.22</v>
       </c>
       <c r="L36" s="25"/>
       <c r="M36" s="25"/>
@@ -1851,7 +1851,7 @@
       </c>
       <c r="B37" s="32">
         <f>K37/K43</f>
-        <v>1.4999999999999999E-2</v>
+        <v>2.1249999999999998E-2</v>
       </c>
       <c r="C37" s="32">
         <v>0</v>
@@ -1875,11 +1875,11 @@
         <v>0</v>
       </c>
       <c r="J37" s="32">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="K37" s="35">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>0.16999999999999998</v>
       </c>
       <c r="L37" s="25"/>
       <c r="M37" s="25"/>
@@ -1973,7 +1973,7 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B40" s="32">
         <f>K40/K43</f>
@@ -2015,11 +2015,11 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B41" s="32">
         <f>K41/K43</f>
-        <v>0.06</v>
+        <v>5.9812500000000005E-2</v>
       </c>
       <c r="C41" s="32">
         <v>0</v>
@@ -2028,7 +2028,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="32">
-        <v>5.0000000000000001E-3</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="F41" s="32">
         <v>0.15</v>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="K41" s="35">
         <f>SUM(C41:J41)</f>
-        <v>0.48</v>
+        <v>0.47850000000000004</v>
       </c>
       <c r="L41" s="25"/>
       <c r="M41" s="25"/>
@@ -2208,7 +2208,7 @@
       </c>
       <c r="B50" s="23">
         <f>B27^(1/A50)</f>
-        <v>0.10625</v>
+        <v>0.10312499999999999</v>
       </c>
       <c r="C50" s="23">
         <f t="shared" ref="C50:E53" si="2">PRODUCT(C27,$A50)</f>
@@ -2228,7 +2228,7 @@
       </c>
       <c r="G50" s="24">
         <f>F50-B50</f>
-        <v>0.54375000000000007</v>
+        <v>0.546875</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2237,7 +2237,7 @@
       </c>
       <c r="B51" s="23">
         <f>B28^(1/A51)</f>
-        <v>0.42635094916407995</v>
+        <v>0.43751700614166367</v>
       </c>
       <c r="C51" s="7">
         <f t="shared" si="2"/>
@@ -2257,7 +2257,7 @@
       </c>
       <c r="G51" s="24">
         <f>F51-B51</f>
-        <v>0.83364905083592</v>
+        <v>0.82248299385833634</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2324,7 +2324,7 @@
       </c>
       <c r="B54" s="7">
         <f>SUM(B50:B53)</f>
-        <v>0.89869970012963629</v>
+        <v>0.90674075710722002</v>
       </c>
       <c r="C54" s="7">
         <f t="shared" ref="C54:E54" si="3">SUM(C50:C53)</f>
@@ -2362,7 +2362,7 @@
       </c>
       <c r="B56" s="7">
         <f>PRODUCT(B54:B55)</f>
-        <v>0.89869970012963629</v>
+        <v>0.90674075710722002</v>
       </c>
       <c r="C56" s="7">
         <f t="shared" ref="C56:E56" si="4">PRODUCT(C54:C55)</f>
@@ -2424,6 +2424,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010006B233B9B3A5024C99847B1D0443027F" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="39a3a9a18fc0038d1c425abb13176a98">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d59a1f78-4cdc-402c-b8a0-58bfb80633d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="635a148d9eedb07babeb6ca05c95a7d9" ns3:_="">
     <xsd:import namespace="d59a1f78-4cdc-402c-b8a0-58bfb80633d0"/>
@@ -2555,35 +2570,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D72B6365-5724-4DCC-8EE2-F84342C5EBFF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F3EA1CF-A27A-4CFA-9674-6A86EB7CE3B7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d59a1f78-4cdc-402c-b8a0-58bfb80633d0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2605,9 +2595,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F3EA1CF-A27A-4CFA-9674-6A86EB7CE3B7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D72B6365-5724-4DCC-8EE2-F84342C5EBFF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d59a1f78-4cdc-402c-b8a0-58bfb80633d0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
new names w/ abbreviation
</commit_message>
<xml_diff>
--- a/problem 3 - concept/jobs.xlsx
+++ b/problem 3 - concept/jobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deric\Desktop\ai-genetic\ai-projet2-genetic\problem 3 - concept\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12929D35-8249-4AA1-85DF-3536C0B512D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D63A9E-3C73-441E-9935-784C5BAF6D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14775" yWindow="2325" windowWidth="23970" windowHeight="14505" xr2:uid="{2134C11B-C8CC-4877-9366-45380615B26B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{2134C11B-C8CC-4877-9366-45380615B26B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -852,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7D3F53-E2D2-416E-AD93-0175C9D788F7}">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,7 +1410,7 @@
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>32</v>
       </c>
@@ -2165,12 +2165,12 @@
       <c r="J44" s="27"/>
       <c r="K44" s="34"/>
     </row>
-    <row r="45" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" ht="120" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>42</v>
       </c>
@@ -2424,21 +2424,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010006B233B9B3A5024C99847B1D0443027F" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="39a3a9a18fc0038d1c425abb13176a98">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d59a1f78-4cdc-402c-b8a0-58bfb80633d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="635a148d9eedb07babeb6ca05c95a7d9" ns3:_="">
     <xsd:import namespace="d59a1f78-4cdc-402c-b8a0-58bfb80633d0"/>
@@ -2570,10 +2555,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F3EA1CF-A27A-4CFA-9674-6A86EB7CE3B7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D72B6365-5724-4DCC-8EE2-F84342C5EBFF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d59a1f78-4cdc-402c-b8a0-58bfb80633d0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2595,19 +2605,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D72B6365-5724-4DCC-8EE2-F84342C5EBFF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F3EA1CF-A27A-4CFA-9674-6A86EB7CE3B7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d59a1f78-4cdc-402c-b8a0-58bfb80633d0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>